<commit_message>
created untracked expenses and completed the functionality of bot
</commit_message>
<xml_diff>
--- a/OLTP tables.xlsx
+++ b/OLTP tables.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiab\Projects\Expense Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C506D13-54E8-42DF-A488-8F17D2CE1099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE9B456-580F-4611-950B-B14D32C6B611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{57EE8AF7-C679-4CBF-87B1-31866FA16C01}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{57EE8AF7-C679-4CBF-87B1-31866FA16C01}"/>
   </bookViews>
   <sheets>
     <sheet name="Expense" sheetId="1" r:id="rId1"/>
     <sheet name="Category" sheetId="3" r:id="rId2"/>
     <sheet name="Source" sheetId="2" r:id="rId3"/>
+    <sheet name="Untracked Expenses" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="186">
   <si>
     <t>expense_id</t>
   </si>
@@ -44,9 +45,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>transaction_id</t>
   </si>
   <si>
@@ -71,15 +69,6 @@
     <t>EX0005</t>
   </si>
   <si>
-    <t>XXXXX0PMEQE</t>
-  </si>
-  <si>
-    <t>XXXXX729NSDF</t>
-  </si>
-  <si>
-    <t>XXXXX73NGTE</t>
-  </si>
-  <si>
     <t>UPI</t>
   </si>
   <si>
@@ -569,18 +558,9 @@
     <t>yes</t>
   </si>
   <si>
-    <t>UTR</t>
-  </si>
-  <si>
-    <t>T2212282313358101152636</t>
-  </si>
-  <si>
     <t>Jharsuguda Trip</t>
   </si>
   <si>
-    <t>T2212290915380238585609</t>
-  </si>
-  <si>
     <t>Travel</t>
   </si>
   <si>
@@ -594,12 +574,36 @@
   </si>
   <si>
     <t>Stay</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Cashless</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -652,15 +656,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -976,246 +981,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59B584A-A2B7-4C59-B1F9-CA5598E04298}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.90625" customWidth="1"/>
-    <col min="11" max="11" width="17.6328125" customWidth="1"/>
-    <col min="12" max="12" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.90625" customWidth="1"/>
+    <col min="10" max="10" width="17.6328125" customWidth="1"/>
+    <col min="11" max="11" width="6.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" s="6">
+        <v>44940.049305555556</v>
+      </c>
+      <c r="C2" s="4">
+        <v>272896038266</v>
+      </c>
+      <c r="D2" s="8">
+        <v>650</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>44940.049305555556</v>
+      </c>
+      <c r="C3" s="4">
+        <v>272903625224</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1900</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>44940.049305555556</v>
+      </c>
+      <c r="C4" s="4">
+        <v>218817727672</v>
+      </c>
+      <c r="D4" s="8">
+        <v>785</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>44939.09375</v>
+      </c>
+      <c r="C5" s="4">
+        <v>300507135625</v>
+      </c>
+      <c r="D5" s="8">
+        <v>22000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" t="s">
+        <v>158</v>
+      </c>
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" t="s">
         <v>171</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4">
-        <v>44923</v>
-      </c>
-      <c r="C2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D2" s="6">
-        <v>272896038266</v>
-      </c>
-      <c r="E2" s="3">
-        <v>650</v>
-      </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>166</v>
-      </c>
-      <c r="I2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" t="s">
-        <v>179</v>
-      </c>
-      <c r="L2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4">
-        <v>44924</v>
-      </c>
-      <c r="C3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D3" s="6">
-        <v>272903625224</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1900</v>
-      </c>
-      <c r="F3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>166</v>
-      </c>
-      <c r="I3" t="s">
-        <v>133</v>
-      </c>
-      <c r="J3" t="s">
-        <v>185</v>
-      </c>
-      <c r="K3" t="s">
-        <v>183</v>
-      </c>
-      <c r="L3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4">
-        <v>44929</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3">
-        <v>785</v>
-      </c>
-      <c r="F4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>167</v>
-      </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" t="s">
-        <v>65</v>
-      </c>
-      <c r="L4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4">
-        <v>44926</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3">
-        <v>22000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J5" t="s">
-        <v>162</v>
-      </c>
-      <c r="K5" t="s">
-        <v>66</v>
-      </c>
-      <c r="L5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B6" s="6">
+        <v>44940.09375</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="8">
+        <v>334.05</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4">
-        <v>44925</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3">
-        <v>334.05</v>
-      </c>
-      <c r="F6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" t="s">
-        <v>54</v>
-      </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="I6" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1230,7 +1225,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
@@ -1242,640 +1237,640 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
         <v>76</v>
-      </c>
-      <c r="C13" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
         <v>83</v>
-      </c>
-      <c r="C20" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
         <v>91</v>
-      </c>
-      <c r="C27" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C38" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B44" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C45" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B48" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C48" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B49" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" t="s">
         <v>127</v>
-      </c>
-      <c r="C49" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B52" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B54" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" t="s">
         <v>133</v>
-      </c>
-      <c r="C55" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B56" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B57" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C57" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C58" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1889,9 +1884,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B12F09-FE8A-4529-936E-7B8535DFF2C1}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1899,204 +1894,204 @@
     <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2">
         <v>45287</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="3">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2">
         <v>33100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2">
         <v>45287</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
         <v>45287</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
+        <v>13098</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="3">
-        <v>13098</v>
-      </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D7" s="3">
-        <v>45287</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="3">
-        <v>45287</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D9" s="3">
+        <v>164</v>
+      </c>
+      <c r="D9" s="2">
         <v>45287</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="3">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2">
         <v>3217</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="2">
+        <v>13098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" s="2">
+        <v>13098</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
         <v>164</v>
       </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="3">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>166</v>
-      </c>
-      <c r="D12" s="3">
-        <v>13098</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13" s="3">
-        <v>13098</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>168</v>
-      </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>13098</v>
       </c>
     </row>
@@ -2112,4 +2107,127 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B19E0E9-F5F6-45F3-AD9D-8D3C653AC3EB}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>44940.049305555556</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="4">
+        <v>218817727672</v>
+      </c>
+      <c r="D2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>44940.049305555556</v>
+      </c>
+      <c r="B3" s="8">
+        <v>5000</v>
+      </c>
+      <c r="C3" s="4">
+        <v>300507135625</v>
+      </c>
+      <c r="D3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>44940.049305555556</v>
+      </c>
+      <c r="B4" s="8">
+        <v>75</v>
+      </c>
+      <c r="C4" s="4">
+        <v>223985882668</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>44939.09375</v>
+      </c>
+      <c r="B5" s="8">
+        <v>54</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>